<commit_message>
CheckCredibility returns a dict object
</commit_message>
<xml_diff>
--- a/Docs/Bias_Score_Analysis/Bias Score.xlsx
+++ b/Docs/Bias_Score_Analysis/Bias Score.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TEXTBLOB" sheetId="3" r:id="rId1"/>
@@ -814,16 +814,16 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1163,11 +1163,11 @@
       <c r="M1" s="22">
         <v>2</v>
       </c>
-      <c r="N1" s="60" t="s">
+      <c r="N1" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -2023,11 +2023,11 @@
       <c r="O1" s="22">
         <v>2</v>
       </c>
-      <c r="P1" s="60" t="s">
+      <c r="P1" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -2941,8 +2941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2955,6 +2955,10 @@
     <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5546875" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -2994,32 +2998,29 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E2" s="17">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="62">
-        <v>-0.5423</v>
-      </c>
-      <c r="H2" s="57" t="s">
-        <v>54</v>
+      <c r="G2" s="60">
+        <v>0.57189999999999996</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>52</v>
       </c>
       <c r="J2" s="53">
-        <v>0.53800000000000003</v>
+        <v>0</v>
       </c>
       <c r="K2" s="53">
-        <v>0.46200000000000002</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="L2" s="53">
-        <v>0</v>
+        <v>0.48099999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -3027,32 +3028,32 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="10">
-        <v>0.39</v>
-      </c>
-      <c r="E3" s="28">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="E3" s="17">
+        <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="62">
-        <v>0.49270000000000003</v>
-      </c>
-      <c r="H3" s="59" t="s">
-        <v>52</v>
+        <v>62</v>
+      </c>
+      <c r="G3" s="60">
+        <v>-0.5423</v>
+      </c>
+      <c r="H3" s="57" t="s">
+        <v>54</v>
       </c>
       <c r="J3" s="53">
-        <v>0</v>
+        <v>0.53800000000000003</v>
       </c>
       <c r="K3" s="53">
-        <v>0.68700000000000006</v>
+        <v>0.46200000000000002</v>
       </c>
       <c r="L3" s="53">
-        <v>0.313</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -3060,17 +3061,20 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="10">
-        <v>1</v>
-      </c>
-      <c r="E4" s="17">
-        <v>1</v>
-      </c>
-      <c r="G4" s="62">
-        <v>0.57189999999999996</v>
+        <v>0.39</v>
+      </c>
+      <c r="E4" s="28">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="60">
+        <v>0.49270000000000003</v>
       </c>
       <c r="H4" s="59" t="s">
         <v>52</v>
@@ -3079,10 +3083,10 @@
         <v>0</v>
       </c>
       <c r="K4" s="53">
-        <v>0.51900000000000002</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="L4" s="53">
-        <v>0.48099999999999998</v>
+        <v>0.313</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -3099,7 +3103,7 @@
       <c r="E5" s="17">
         <v>0.6</v>
       </c>
-      <c r="G5" s="62">
+      <c r="G5" s="60">
         <v>0</v>
       </c>
       <c r="H5" s="49" t="s">
@@ -3129,7 +3133,7 @@
       <c r="E6" s="15">
         <v>0</v>
       </c>
-      <c r="G6" s="62">
+      <c r="G6" s="60">
         <v>0.2263</v>
       </c>
       <c r="H6" s="59" t="s">
@@ -3162,28 +3166,28 @@
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="65" t="s">
+      <c r="B21" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="65" t="s">
+      <c r="B23" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3196,8 +3200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3207,154 +3211,154 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="61" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="62" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="62" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="62" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="62" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="62" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="62" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="62" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="62" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="62" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="62" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="62" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="62" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="64" t="s">
+      <c r="A13" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="62" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="64" t="s">
+      <c r="A14" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="62" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="62" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="62" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="62" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="64" t="s">
+      <c r="A18" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="62" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="64" t="s">
+      <c r="A19" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="62" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created Bias Score folder under docs plus SPACY tests
</commit_message>
<xml_diff>
--- a/Docs/Bias_Score_Analysis/Bias Score.xlsx
+++ b/Docs/Bias_Score_Analysis/Bias Score.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="TEXTBLOB" sheetId="3" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="113">
   <si>
     <t>Website</t>
   </si>
@@ -195,12 +195,6 @@
     <t>FINAL BIAS (POL *SUBJ)</t>
   </si>
   <si>
-    <t>SUBJ</t>
-  </si>
-  <si>
-    <t>OBJ</t>
-  </si>
-  <si>
     <t>CHECK CREDIBILITY</t>
   </si>
   <si>
@@ -285,9 +279,6 @@
     <t>https://metro.co.uk/2020/10/04/boris-johnson-admits-eat-out-to-help-out-could-have-helped-spread-covid-13370357/</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
     <t>NEUTRAL</t>
   </si>
   <si>
@@ -457,6 +448,12 @@
   </si>
   <si>
     <t>code "namedEntityRecognition(url, tag)"</t>
+  </si>
+  <si>
+    <t>ABS(POL*SUB)</t>
+  </si>
+  <si>
+    <t>Subjectiv</t>
   </si>
 </sst>
 </file>
@@ -554,7 +551,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -630,6 +627,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -731,7 +734,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -747,14 +750,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -767,8 +766,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -818,6 +815,46 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1105,626 +1142,648 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView zoomScale="95" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" customWidth="1"/>
-    <col min="14" max="14" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" hidden="1" customWidth="1"/>
+    <col min="9" max="11" width="8.88671875" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="33" t="s">
+      <c r="E1" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="22">
-        <v>-2</v>
-      </c>
-      <c r="J1" s="22">
-        <v>-1</v>
-      </c>
-      <c r="K1" s="22">
-        <v>0</v>
-      </c>
-      <c r="L1" s="22">
+      <c r="I1" s="63">
+        <v>0</v>
+      </c>
+      <c r="J1" s="63">
+        <v>0.5</v>
+      </c>
+      <c r="K1" s="63">
         <v>1</v>
       </c>
-      <c r="M1" s="22">
-        <v>2</v>
-      </c>
-      <c r="N1" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L1" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="66">
         <v>-1</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="66">
         <v>1</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="17">
+      <c r="F2" s="77">
+        <f>ABS(D2*E2)</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="67">
         <f>IF(E2&lt;0.5, E2, E2*2)</f>
         <v>2</v>
       </c>
-      <c r="H2" s="19">
+      <c r="H2" s="68">
         <f t="shared" ref="H2:H15" si="0">D2*G2</f>
         <v>-2</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="46"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="66">
         <v>1</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="66">
         <v>0.3</v>
       </c>
-      <c r="F3" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="28">
-        <f t="shared" ref="G3:G15" si="1">IF(E3&lt;0.5, E3, E3*2)</f>
+      <c r="F3" s="77">
+        <f t="shared" ref="F3:F7" si="1">ABS(D3*E3)</f>
         <v>0.3</v>
       </c>
-      <c r="H3" s="19">
+      <c r="G3" s="71">
+        <f t="shared" ref="G3:G15" si="2">IF(E3&lt;0.5, E3, E3*2)</f>
+        <v>0.3</v>
+      </c>
+      <c r="H3" s="68">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="46"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I3" s="69"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="66">
         <v>0.39</v>
       </c>
-      <c r="E4" s="28">
-        <v>0</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="28">
+      <c r="E4" s="66">
+        <v>0</v>
+      </c>
+      <c r="F4" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H4" s="19">
+      <c r="G4" s="71">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="46"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I4" s="69"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="66">
         <v>1</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="66">
         <v>1</v>
       </c>
-      <c r="F5" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="17">
+      <c r="F5" s="77">
         <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G5" s="67">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="68">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="46"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="56"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="10">
-        <v>0</v>
-      </c>
-      <c r="E6" s="17">
+      <c r="D6" s="66">
+        <v>0</v>
+      </c>
+      <c r="E6" s="66">
         <v>0.6</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="17">
+      <c r="F6" s="77">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="67">
+        <f t="shared" si="2"/>
         <v>1.2</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="46"/>
-    </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I6" s="69"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="10">
-        <v>0</v>
-      </c>
-      <c r="E7" s="15">
-        <v>0</v>
-      </c>
-      <c r="F7" s="16" t="s">
+      <c r="D7" s="66">
+        <v>0</v>
+      </c>
+      <c r="E7" s="66">
+        <v>0</v>
+      </c>
+      <c r="F7" s="77">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="71">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="68">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="69"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="O7" s="40" t="s">
+      <c r="N7" s="74" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>1</v>
+      </c>
+      <c r="B8" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="76">
+        <v>-1.3959686147186101E-2</v>
+      </c>
+      <c r="E8" s="76">
+        <v>0.43129437229437201</v>
+      </c>
+      <c r="F8" s="77">
+        <f>ABS(D8*E8)</f>
+        <v>6.0207340742770695E-3</v>
+      </c>
+      <c r="G8" s="78">
+        <f t="shared" si="2"/>
+        <v>0.43129437229437201</v>
+      </c>
+      <c r="H8" s="68">
+        <f>D8*G8</f>
+        <v>-6.0207340742770695E-3</v>
+      </c>
+      <c r="I8" s="69"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="79">
+        <v>49.5</v>
+      </c>
+      <c r="M8" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="P7" s="40" t="s">
+      <c r="N8" s="70" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="12">
-        <v>1</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="14">
-        <v>-1.3959686147186101E-2</v>
-      </c>
-      <c r="E8" s="29">
-        <v>0.43129437229437201</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="29">
-        <f t="shared" si="1"/>
-        <v>0.43129437229437201</v>
-      </c>
-      <c r="H8" s="32">
-        <f t="shared" si="0"/>
-        <v>-6.0207340742770695E-3</v>
-      </c>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="43">
-        <v>49.5</v>
-      </c>
-      <c r="O8" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="P8" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="76">
         <v>5.5258047508047498E-2</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="76">
         <v>0.43147743922743897</v>
       </c>
-      <c r="G9" s="11">
-        <f t="shared" si="1"/>
+      <c r="F9" s="77">
+        <f t="shared" ref="F9:F15" si="3">ABS(D9*E9)</f>
+        <v>2.3842600835480499E-2</v>
+      </c>
+      <c r="G9" s="78">
+        <f t="shared" si="2"/>
         <v>0.43147743922743897</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="68">
         <f t="shared" si="0"/>
         <v>2.3842600835480499E-2</v>
       </c>
-      <c r="I9" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="44">
+      <c r="I9" s="69"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="81">
         <v>95</v>
       </c>
-      <c r="O9" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="P9" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M9" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="N9" s="73" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="6">
+      <c r="C10" s="80" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="76">
         <v>0.203059861285667</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="76">
         <v>0.50926139272913395</v>
       </c>
-      <c r="G10" s="17">
-        <f t="shared" si="1"/>
+      <c r="F10" s="77">
+        <f t="shared" si="3"/>
+        <v>0.10341054776572353</v>
+      </c>
+      <c r="G10" s="67">
+        <f t="shared" si="2"/>
         <v>1.0185227854582679</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="68">
         <f t="shared" si="0"/>
         <v>0.20682109553144706</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="45">
+      <c r="I10" s="69"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="79">
         <v>82.5</v>
       </c>
-      <c r="O10" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="P10" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M10" s="70" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="70" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="B11" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="75" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="76">
         <v>8.2133490344480198E-2</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="76">
         <v>0.41494910756655701</v>
       </c>
-      <c r="G11" s="11">
-        <f t="shared" si="1"/>
+      <c r="F11" s="77">
+        <f t="shared" si="3"/>
+        <v>3.4081218519768482E-2</v>
+      </c>
+      <c r="G11" s="78">
+        <f t="shared" si="2"/>
         <v>0.41494910756655701</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="68">
         <f t="shared" si="0"/>
         <v>3.4081218519768482E-2</v>
       </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="44">
+      <c r="I11" s="69"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="81">
         <v>100</v>
       </c>
-      <c r="O11" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="P11" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="25">
+      <c r="M11" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="N11" s="73" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="21">
         <v>5</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="76">
         <v>7.5195158871629406E-2</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="76">
         <v>0.54452720663504905</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="17">
-        <f t="shared" si="1"/>
+      <c r="F12" s="77">
+        <f t="shared" si="3"/>
+        <v>4.0945809812847088E-2</v>
+      </c>
+      <c r="G12" s="67">
+        <f t="shared" si="2"/>
         <v>1.0890544132700981</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="68">
         <f t="shared" si="0"/>
         <v>8.1891619625694176E-2</v>
       </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="45">
+      <c r="I12" s="69"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="79">
         <v>95</v>
       </c>
-      <c r="O12" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="P12" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="41">
+      <c r="M12" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="N12" s="70" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="35">
         <v>6</v>
       </c>
-      <c r="B13" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="6">
+      <c r="B13" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="75" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="76">
         <v>-0.113888888888888</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="76">
         <v>0.65277777777777701</v>
       </c>
-      <c r="G13" s="17">
-        <f t="shared" si="1"/>
+      <c r="F13" s="77">
+        <f t="shared" si="3"/>
+        <v>7.4344135802468472E-2</v>
+      </c>
+      <c r="G13" s="67">
+        <f t="shared" si="2"/>
         <v>1.305555555555554</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="68">
         <f t="shared" si="0"/>
         <v>-0.14868827160493694</v>
       </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="44">
+      <c r="I13" s="69"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="72"/>
+      <c r="L13" s="81">
         <v>100</v>
       </c>
-      <c r="O13" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="P13" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="41">
+      <c r="M13" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="N13" s="73" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="35">
         <v>7</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="82" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="6">
+      <c r="D14" s="76">
         <v>0.14939723320158099</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="76">
         <v>0.37066205533596802</v>
       </c>
-      <c r="G14" s="11">
-        <f t="shared" si="1"/>
+      <c r="F14" s="77">
+        <f t="shared" si="3"/>
+        <v>5.5375885520004935E-2</v>
+      </c>
+      <c r="G14" s="78">
+        <f t="shared" si="2"/>
         <v>0.37066205533596802</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="68">
         <f t="shared" si="0"/>
         <v>5.5375885520004935E-2</v>
       </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="45">
+      <c r="I14" s="69"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="79">
         <v>75</v>
       </c>
-      <c r="O14" s="20" t="s">
+      <c r="M14" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="N14" s="70" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="35">
+        <v>8</v>
+      </c>
+      <c r="B15" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="P14" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="41">
-        <v>8</v>
-      </c>
-      <c r="B15" s="41" t="s">
+      <c r="C15" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="6">
+      <c r="D15" s="76">
         <v>1.4011491728883E-2</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="76">
         <v>0.38156382667252198</v>
       </c>
-      <c r="G15" s="11">
-        <f t="shared" si="1"/>
+      <c r="F15" s="77">
+        <f t="shared" si="3"/>
+        <v>5.3462784014629882E-3</v>
+      </c>
+      <c r="G15" s="78">
+        <f t="shared" si="2"/>
         <v>0.38156382667252198</v>
       </c>
-      <c r="H15" s="19">
+      <c r="H15" s="68">
         <f t="shared" si="0"/>
         <v>5.3462784014629882E-3</v>
       </c>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="44">
+      <c r="I15" s="69"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="72"/>
+      <c r="L15" s="81">
         <v>100</v>
       </c>
-      <c r="O15" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="P15" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M15" s="73" t="s">
+        <v>42</v>
+      </c>
+      <c r="N15" s="73" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C17" s="2"/>
-      <c r="O17" s="31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F18" s="6">
+        <f>SUM(F8:F15)</f>
+        <v>0.34336721073203308</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C19" s="2"/>
-      <c r="I19" s="37">
+      <c r="F19">
+        <f>F18/8</f>
+        <v>4.2920901341504135E-2</v>
+      </c>
+      <c r="I19" s="31">
         <v>-1</v>
       </c>
-      <c r="J19" s="35">
-        <v>0</v>
-      </c>
-      <c r="K19" s="38" t="s">
+      <c r="J19" s="29">
+        <v>0</v>
+      </c>
+      <c r="K19" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="L19" s="36" t="s">
+      <c r="L19" s="30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20" s="2"/>
@@ -1735,9 +1794,8 @@
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20"/>
-      <c r="M20"/>
-    </row>
-    <row r="21" spans="1:15" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:12" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21" s="2"/>
@@ -1745,18 +1803,17 @@
       <c r="G21"/>
       <c r="H21"/>
       <c r="I21"/>
-      <c r="J21" s="37">
-        <v>0</v>
-      </c>
-      <c r="K21" s="38" t="s">
+      <c r="J21" s="31">
+        <v>0</v>
+      </c>
+      <c r="K21" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="L21" s="36" t="s">
+      <c r="L21" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="M21"/>
-    </row>
-    <row r="22" spans="1:15" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:12" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22" s="2"/>
@@ -1767,9 +1824,8 @@
       <c r="J22"/>
       <c r="K22"/>
       <c r="L22"/>
-      <c r="M22"/>
-    </row>
-    <row r="23" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23" s="2"/>
@@ -1777,14 +1833,13 @@
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
-      <c r="J23" s="39" t="s">
+      <c r="J23" s="33" t="s">
         <v>24</v>
       </c>
       <c r="K23"/>
       <c r="L23"/>
-      <c r="M23"/>
-    </row>
-    <row r="24" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24" s="2"/>
@@ -1792,14 +1847,13 @@
       <c r="G24"/>
       <c r="H24"/>
       <c r="I24"/>
-      <c r="J24" s="39" t="s">
+      <c r="J24" s="33" t="s">
         <v>23</v>
       </c>
       <c r="K24"/>
       <c r="L24"/>
-      <c r="M24"/>
-    </row>
-    <row r="25" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25" s="2"/>
@@ -1809,10 +1863,8 @@
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
-      <c r="L25"/>
-      <c r="M25"/>
-    </row>
-    <row r="26" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26" s="2"/>
@@ -1822,10 +1874,8 @@
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
-      <c r="L26"/>
-      <c r="M26"/>
-    </row>
-    <row r="27" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27" s="2"/>
@@ -1835,10 +1885,8 @@
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
-      <c r="L27"/>
-      <c r="M27"/>
-    </row>
-    <row r="28" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28" s="2"/>
@@ -1848,10 +1896,8 @@
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
-      <c r="L28"/>
-      <c r="M28"/>
-    </row>
-    <row r="29" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29" s="2"/>
@@ -1861,10 +1907,8 @@
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
-      <c r="L29"/>
-      <c r="M29"/>
-    </row>
-    <row r="30" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30" s="2"/>
@@ -1874,10 +1918,8 @@
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
-      <c r="L30"/>
-      <c r="M30"/>
-    </row>
-    <row r="31" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31" s="2"/>
@@ -1887,10 +1929,8 @@
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
-      <c r="L31"/>
-      <c r="M31"/>
-    </row>
-    <row r="33" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33" s="2"/>
@@ -1900,10 +1940,8 @@
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
-      <c r="L33"/>
-      <c r="M33"/>
-    </row>
-    <row r="34" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34" s="2"/>
@@ -1913,10 +1951,8 @@
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
-      <c r="L34"/>
-      <c r="M34"/>
-    </row>
-    <row r="35" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35" s="2"/>
@@ -1926,12 +1962,10 @@
       <c r="I35"/>
       <c r="J35"/>
       <c r="K35"/>
-      <c r="L35"/>
-      <c r="M35"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="L1:N1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1"/>
@@ -1987,47 +2021,47 @@
       <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="G1" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="52" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="33" t="s">
+      <c r="H1" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="48" t="s">
-        <v>53</v>
-      </c>
       <c r="I1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J1" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="K1" s="22">
+        <v>56</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="18">
         <v>-2</v>
       </c>
-      <c r="L1" s="22">
+      <c r="L1" s="18">
         <v>-1</v>
       </c>
-      <c r="M1" s="22">
-        <v>0</v>
-      </c>
-      <c r="N1" s="22">
+      <c r="M1" s="18">
+        <v>0</v>
+      </c>
+      <c r="N1" s="18">
         <v>1</v>
       </c>
-      <c r="O1" s="22">
+      <c r="O1" s="18">
         <v>2</v>
       </c>
-      <c r="P1" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
+      <c r="P1" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -2039,34 +2073,34 @@
       <c r="C2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="53">
+      <c r="D2" s="47">
         <v>0.53800000000000003</v>
       </c>
-      <c r="E2" s="53">
+      <c r="E2" s="47">
         <v>0.46200000000000002</v>
       </c>
-      <c r="F2" s="53">
-        <v>0</v>
-      </c>
-      <c r="G2" s="53">
+      <c r="F2" s="47">
+        <v>0</v>
+      </c>
+      <c r="G2" s="47">
         <v>-0.5423</v>
       </c>
-      <c r="H2" s="57" t="s">
-        <v>54</v>
+      <c r="H2" s="51" t="s">
+        <v>52</v>
       </c>
       <c r="I2" s="10">
         <v>-1</v>
       </c>
-      <c r="J2" s="19">
+      <c r="J2" s="15">
         <f t="shared" ref="J2:J15" si="0">F2*I2</f>
         <v>0</v>
       </c>
       <c r="K2" s="7"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="46"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="40"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
@@ -2078,34 +2112,34 @@
       <c r="C3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="53">
-        <v>0</v>
-      </c>
-      <c r="E3" s="53">
+      <c r="D3" s="47">
+        <v>0</v>
+      </c>
+      <c r="E3" s="47">
         <v>0.625</v>
       </c>
-      <c r="F3" s="53">
+      <c r="F3" s="47">
         <v>0.375</v>
       </c>
-      <c r="G3" s="53">
+      <c r="G3" s="47">
         <v>0.63690000000000002</v>
       </c>
-      <c r="H3" s="59" t="s">
-        <v>52</v>
+      <c r="H3" s="53" t="s">
+        <v>50</v>
       </c>
       <c r="I3" s="10">
         <v>1</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="15">
         <f t="shared" si="0"/>
         <v>0.375</v>
       </c>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
       <c r="N3" s="7"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="46"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="40"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
@@ -2117,34 +2151,34 @@
       <c r="C4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="53">
-        <v>0</v>
-      </c>
-      <c r="E4" s="53">
+      <c r="D4" s="47">
+        <v>0</v>
+      </c>
+      <c r="E4" s="47">
         <v>0.68700000000000006</v>
       </c>
-      <c r="F4" s="53">
+      <c r="F4" s="47">
         <v>0.313</v>
       </c>
-      <c r="G4" s="53">
+      <c r="G4" s="47">
         <v>0.49270000000000003</v>
       </c>
-      <c r="H4" s="59" t="s">
-        <v>52</v>
+      <c r="H4" s="53" t="s">
+        <v>50</v>
       </c>
       <c r="I4" s="10">
         <v>0.39</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="15">
         <f t="shared" si="0"/>
         <v>0.12207</v>
       </c>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
       <c r="M4" s="7"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="46"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="40"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
@@ -2156,34 +2190,34 @@
       <c r="C5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="53">
-        <v>0</v>
-      </c>
-      <c r="E5" s="53">
+      <c r="D5" s="47">
+        <v>0</v>
+      </c>
+      <c r="E5" s="47">
         <v>0.51900000000000002</v>
       </c>
-      <c r="F5" s="53">
+      <c r="F5" s="47">
         <v>0.48099999999999998</v>
       </c>
-      <c r="G5" s="53">
+      <c r="G5" s="47">
         <v>0.57189999999999996</v>
       </c>
-      <c r="H5" s="59" t="s">
-        <v>52</v>
+      <c r="H5" s="53" t="s">
+        <v>50</v>
       </c>
       <c r="I5" s="10">
         <v>1</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="15">
         <f t="shared" si="0"/>
         <v>0.48099999999999998</v>
       </c>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
       <c r="O5" s="7"/>
-      <c r="P5" s="46"/>
+      <c r="P5" s="40"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
@@ -2195,34 +2229,34 @@
       <c r="C6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="53">
-        <v>0</v>
-      </c>
-      <c r="E6" s="53">
+      <c r="D6" s="47">
+        <v>0</v>
+      </c>
+      <c r="E6" s="47">
         <v>1</v>
       </c>
-      <c r="F6" s="53">
-        <v>0</v>
-      </c>
-      <c r="G6" s="53">
-        <v>0</v>
-      </c>
-      <c r="H6" s="49" t="s">
-        <v>57</v>
+      <c r="F6" s="47">
+        <v>0</v>
+      </c>
+      <c r="G6" s="47">
+        <v>0</v>
+      </c>
+      <c r="H6" s="43" t="s">
+        <v>54</v>
       </c>
       <c r="I6" s="10">
         <v>0</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
       <c r="M6" s="7"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="46"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="40"/>
     </row>
     <row r="7" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
@@ -2234,88 +2268,88 @@
       <c r="C7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="53">
-        <v>0</v>
-      </c>
-      <c r="E7" s="53">
+      <c r="D7" s="47">
+        <v>0</v>
+      </c>
+      <c r="E7" s="47">
         <v>0.84</v>
       </c>
-      <c r="F7" s="53">
+      <c r="F7" s="47">
         <v>0.16</v>
       </c>
-      <c r="G7" s="53">
+      <c r="G7" s="47">
         <v>0.2263</v>
       </c>
-      <c r="H7" s="59" t="s">
-        <v>52</v>
+      <c r="H7" s="53" t="s">
+        <v>50</v>
       </c>
       <c r="I7" s="10">
         <v>0</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
       <c r="M7" s="7"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q7" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="R7" s="40" t="s">
-        <v>30</v>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q7" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="R7" s="34" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="54">
+      <c r="A8" s="48">
         <v>1</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="56">
+      <c r="D8" s="50">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="E8" s="56">
+      <c r="E8" s="50">
         <v>0.82</v>
       </c>
-      <c r="F8" s="56">
+      <c r="F8" s="50">
         <v>0.122</v>
       </c>
-      <c r="G8" s="56">
+      <c r="G8" s="50">
         <v>0.98270000000000002</v>
       </c>
-      <c r="H8" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="I8" s="14">
+      <c r="H8" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="12">
         <v>-1.3959686147186101E-2</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="26">
         <f t="shared" si="0"/>
         <v>-1.7030817099567043E-3</v>
       </c>
-      <c r="K8" s="23"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="43">
+      <c r="K8" s="19"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="37">
         <v>49.5</v>
       </c>
-      <c r="Q8" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="R8" s="23" t="s">
-        <v>32</v>
+      <c r="Q8" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8" s="19" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -2326,43 +2360,43 @@
         <v>3</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="53">
+        <v>55</v>
+      </c>
+      <c r="D9" s="47">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="E9" s="53">
+      <c r="E9" s="47">
         <v>0.86199999999999999</v>
       </c>
-      <c r="F9" s="53">
+      <c r="F9" s="47">
         <v>6.2E-2</v>
       </c>
-      <c r="G9" s="53">
+      <c r="G9" s="47">
         <v>-0.9819</v>
       </c>
-      <c r="H9" s="57" t="s">
-        <v>54</v>
+      <c r="H9" s="51" t="s">
+        <v>52</v>
       </c>
       <c r="I9" s="6">
         <v>5.5258047508047498E-2</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="15">
         <f t="shared" si="0"/>
         <v>3.4259989454989447E-3</v>
       </c>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
       <c r="N9" s="7"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="44">
+      <c r="O9" s="17"/>
+      <c r="P9" s="38">
         <v>95</v>
       </c>
-      <c r="Q9" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="R9" s="31" t="s">
-        <v>32</v>
+      <c r="Q9" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="R9" s="25" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -2373,43 +2407,43 @@
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="53">
+        <v>53</v>
+      </c>
+      <c r="D10" s="47">
         <v>2.7E-2</v>
       </c>
-      <c r="E10" s="53">
+      <c r="E10" s="47">
         <v>0.92300000000000004</v>
       </c>
-      <c r="F10" s="53">
+      <c r="F10" s="47">
         <v>0.05</v>
       </c>
-      <c r="G10" s="53">
+      <c r="G10" s="47">
         <v>0.89629999999999999</v>
       </c>
-      <c r="H10" s="59" t="s">
-        <v>52</v>
+      <c r="H10" s="53" t="s">
+        <v>50</v>
       </c>
       <c r="I10" s="6">
         <v>0.203059861285667</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="15">
         <f t="shared" si="0"/>
         <v>1.015299306428335E-2</v>
       </c>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
       <c r="N10" s="7"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="45">
+      <c r="O10" s="16"/>
+      <c r="P10" s="39">
         <v>82.5</v>
       </c>
-      <c r="Q10" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="R10" s="20" t="s">
-        <v>32</v>
+      <c r="Q10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="R10" s="16" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -2417,268 +2451,268 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="53">
+        <v>32</v>
+      </c>
+      <c r="D11" s="47">
         <v>0.112</v>
       </c>
-      <c r="E11" s="53">
+      <c r="E11" s="47">
         <v>0.81200000000000006</v>
       </c>
-      <c r="F11" s="53">
+      <c r="F11" s="47">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="G11" s="53">
+      <c r="G11" s="47">
         <v>-0.99660000000000004</v>
       </c>
-      <c r="H11" s="57" t="s">
-        <v>54</v>
+      <c r="H11" s="51" t="s">
+        <v>52</v>
       </c>
       <c r="I11" s="6">
         <v>8.2133490344480198E-2</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="15">
         <f t="shared" si="0"/>
         <v>6.3242787565249755E-3</v>
       </c>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
       <c r="N11" s="7"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="44">
+      <c r="O11" s="17"/>
+      <c r="P11" s="38">
         <v>100</v>
       </c>
-      <c r="Q11" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="R11" s="31" t="s">
-        <v>32</v>
+      <c r="Q11" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="R11" s="25" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="25">
+      <c r="A12" s="21">
         <v>5</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="53">
+      <c r="D12" s="47">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="E12" s="53">
+      <c r="E12" s="47">
         <v>0.77900000000000003</v>
       </c>
-      <c r="F12" s="53">
+      <c r="F12" s="47">
         <v>0.128</v>
       </c>
-      <c r="G12" s="53">
+      <c r="G12" s="47">
         <v>0.99790000000000001</v>
       </c>
-      <c r="H12" s="59" t="s">
-        <v>52</v>
+      <c r="H12" s="53" t="s">
+        <v>50</v>
       </c>
       <c r="I12" s="6">
         <v>7.5195158871629406E-2</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="15">
         <f t="shared" si="0"/>
         <v>9.6249803355685642E-3</v>
       </c>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="45">
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="39">
         <v>95</v>
       </c>
-      <c r="Q12" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="R12" s="20" t="s">
-        <v>32</v>
+      <c r="Q12" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="R12" s="16" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="41">
+      <c r="A13" s="35">
         <v>6</v>
       </c>
-      <c r="B13" s="41" t="s">
-        <v>37</v>
+      <c r="B13" s="35" t="s">
+        <v>35</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="53">
+        <v>36</v>
+      </c>
+      <c r="D13" s="47">
         <v>0.09</v>
       </c>
-      <c r="E13" s="53">
+      <c r="E13" s="47">
         <v>0.76</v>
       </c>
-      <c r="F13" s="53">
+      <c r="F13" s="47">
         <v>0.14899999999999999</v>
       </c>
-      <c r="G13" s="53">
+      <c r="G13" s="47">
         <v>0.93859999999999999</v>
       </c>
-      <c r="H13" s="59" t="s">
-        <v>52</v>
+      <c r="H13" s="53" t="s">
+        <v>50</v>
       </c>
       <c r="I13" s="6">
         <v>-0.113888888888888</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J13" s="15">
         <f t="shared" si="0"/>
         <v>-1.6969444444444311E-2</v>
       </c>
-      <c r="K13" s="21"/>
+      <c r="K13" s="17"/>
       <c r="L13" s="7"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="44">
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="38">
         <v>100</v>
       </c>
-      <c r="Q13" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="R13" s="31" t="s">
-        <v>32</v>
+      <c r="Q13" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="R13" s="25" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="41">
+      <c r="A14" s="35">
         <v>7</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="53">
+      <c r="D14" s="47">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="E14" s="53">
+      <c r="E14" s="47">
         <v>0.85599999999999998</v>
       </c>
-      <c r="F14" s="53">
+      <c r="F14" s="47">
         <v>0.109</v>
       </c>
-      <c r="G14" s="53">
+      <c r="G14" s="47">
         <v>0.995</v>
       </c>
-      <c r="H14" s="59" t="s">
-        <v>52</v>
+      <c r="H14" s="53" t="s">
+        <v>50</v>
       </c>
       <c r="I14" s="6">
         <v>0.14939723320158099</v>
       </c>
-      <c r="J14" s="19">
+      <c r="J14" s="15">
         <f t="shared" si="0"/>
         <v>1.6284298418972328E-2</v>
       </c>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
       <c r="N14" s="7"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="45">
+      <c r="O14" s="16"/>
+      <c r="P14" s="39">
         <v>75</v>
       </c>
-      <c r="Q14" s="20" t="s">
+      <c r="Q14" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="R14" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="35">
+        <v>8</v>
+      </c>
+      <c r="B15" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="R14" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="41">
-        <v>8</v>
-      </c>
-      <c r="B15" s="41" t="s">
+      <c r="C15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="53">
+      <c r="D15" s="47">
         <v>0.123</v>
       </c>
-      <c r="E15" s="53">
+      <c r="E15" s="47">
         <v>0.754</v>
       </c>
-      <c r="F15" s="53">
+      <c r="F15" s="47">
         <v>0.122</v>
       </c>
-      <c r="G15" s="53">
+      <c r="G15" s="47">
         <v>-0.6915</v>
       </c>
-      <c r="H15" s="57" t="s">
-        <v>54</v>
+      <c r="H15" s="51" t="s">
+        <v>52</v>
       </c>
       <c r="I15" s="6">
         <v>1.4011491728883E-2</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J15" s="15">
         <f t="shared" si="0"/>
         <v>1.709401990923726E-3</v>
       </c>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
       <c r="N15" s="7"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="44">
+      <c r="O15" s="17"/>
+      <c r="P15" s="38">
         <v>100</v>
       </c>
-      <c r="Q15" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="R15" s="31" t="s">
-        <v>32</v>
+      <c r="Q15" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="R15" s="25" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C16" s="2"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C17" s="2"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="Q17" s="31" t="s">
-        <v>47</v>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="Q17" s="25" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C18" s="2"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C19" s="2"/>
@@ -2941,7 +2975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
@@ -2966,31 +3000,31 @@
         <v>19</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="46" t="s">
         <v>48</v>
-      </c>
-      <c r="K1" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" s="52" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -2998,28 +3032,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10">
         <v>1</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="14">
         <v>1</v>
       </c>
-      <c r="G2" s="60">
+      <c r="G2" s="54">
         <v>0.57189999999999996</v>
       </c>
-      <c r="H2" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="53">
-        <v>0</v>
-      </c>
-      <c r="K2" s="53">
+      <c r="H2" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="47">
+        <v>0</v>
+      </c>
+      <c r="K2" s="47">
         <v>0.51900000000000002</v>
       </c>
-      <c r="L2" s="53">
+      <c r="L2" s="47">
         <v>0.48099999999999998</v>
       </c>
     </row>
@@ -3028,31 +3062,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="10">
         <v>-1</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="14">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="60">
+        <v>59</v>
+      </c>
+      <c r="G3" s="54">
         <v>-0.5423</v>
       </c>
-      <c r="H3" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="J3" s="53">
+      <c r="H3" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="47">
         <v>0.53800000000000003</v>
       </c>
-      <c r="K3" s="53">
+      <c r="K3" s="47">
         <v>0.46200000000000002</v>
       </c>
-      <c r="L3" s="53">
+      <c r="L3" s="47">
         <v>0</v>
       </c>
     </row>
@@ -3061,31 +3095,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="10">
         <v>0.39</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="24">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" s="60">
+        <v>60</v>
+      </c>
+      <c r="G4" s="54">
         <v>0.49270000000000003</v>
       </c>
-      <c r="H4" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="J4" s="53">
-        <v>0</v>
-      </c>
-      <c r="K4" s="53">
+      <c r="H4" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="47">
+        <v>0</v>
+      </c>
+      <c r="K4" s="47">
         <v>0.68700000000000006</v>
       </c>
-      <c r="L4" s="53">
+      <c r="L4" s="47">
         <v>0.313</v>
       </c>
     </row>
@@ -3094,28 +3128,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="10">
         <v>0</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="14">
         <v>0.6</v>
       </c>
-      <c r="G5" s="60">
-        <v>0</v>
-      </c>
-      <c r="H5" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="J5" s="53">
-        <v>0</v>
-      </c>
-      <c r="K5" s="53">
+      <c r="G5" s="54">
+        <v>0</v>
+      </c>
+      <c r="H5" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="47">
+        <v>0</v>
+      </c>
+      <c r="K5" s="47">
         <v>1</v>
       </c>
-      <c r="L5" s="53">
+      <c r="L5" s="47">
         <v>0</v>
       </c>
     </row>
@@ -3124,70 +3158,70 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="10">
         <v>0</v>
       </c>
-      <c r="E6" s="15">
-        <v>0</v>
-      </c>
-      <c r="G6" s="60">
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="G6" s="54">
         <v>0.2263</v>
       </c>
-      <c r="H6" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" s="53">
-        <v>0</v>
-      </c>
-      <c r="K6" s="53">
+      <c r="H6" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="47">
+        <v>0</v>
+      </c>
+      <c r="K6" s="47">
         <v>0.84</v>
       </c>
-      <c r="L6" s="53">
+      <c r="L6" s="47">
         <v>0.16</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="63" t="s">
-        <v>111</v>
-      </c>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
+      <c r="B21" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="63" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
+      <c r="B22" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="63" t="s">
-        <v>113</v>
-      </c>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
+      <c r="B23" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3211,155 +3245,155 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="61" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="56" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="62" t="s">
+      <c r="B3" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="62" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="56" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="62" t="s">
+      <c r="B4" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="62" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="56" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="62" t="s">
+      <c r="B5" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="62" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="56" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="62" t="s">
+      <c r="B6" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="62" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="56" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="62" t="s">
+      <c r="B7" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="62" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="56" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="62" t="s">
+      <c r="B8" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="62" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="56" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="62" t="s">
+      <c r="B9" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="62" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="56" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="62" t="s">
+      <c r="B10" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="62" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="56" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="62" t="s">
+      <c r="B11" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="62" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="56" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="62" t="s">
+      <c r="B12" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="62" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="56" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="62" t="s">
+      <c r="B13" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="62" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="56" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="62" t="s">
+      <c r="B14" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="62" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="56" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="62" t="s">
+      <c r="B15" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="62" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="56" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="62" t="s">
+      <c r="B16" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="62" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="56" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="62" t="s">
+      <c r="B17" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="62" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="56" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="62" t="s">
+      <c r="B18" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="62" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="56" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="62" t="s">
+      <c r="B19" s="56" t="s">
         <v>107</v>
-      </c>
-      <c r="B18" s="62" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="62" t="s">
-        <v>109</v>
-      </c>
-      <c r="B19" s="62" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created Bias Score folder under docs + SPACY tests
</commit_message>
<xml_diff>
--- a/Docs/Bias_Score_Analysis/Bias Score.xlsx
+++ b/Docs/Bias_Score_Analysis/Bias Score.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="TEXTBLOB" sheetId="3" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="113">
   <si>
     <t>Website</t>
   </si>
@@ -195,12 +195,6 @@
     <t>FINAL BIAS (POL *SUBJ)</t>
   </si>
   <si>
-    <t>SUBJ</t>
-  </si>
-  <si>
-    <t>OBJ</t>
-  </si>
-  <si>
     <t>CHECK CREDIBILITY</t>
   </si>
   <si>
@@ -285,9 +279,6 @@
     <t>https://metro.co.uk/2020/10/04/boris-johnson-admits-eat-out-to-help-out-could-have-helped-spread-covid-13370357/</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
     <t>NEUTRAL</t>
   </si>
   <si>
@@ -457,6 +448,12 @@
   </si>
   <si>
     <t>code "namedEntityRecognition(url, tag)"</t>
+  </si>
+  <si>
+    <t>ABS(POL*SUB)</t>
+  </si>
+  <si>
+    <t>Subjectiv</t>
   </si>
 </sst>
 </file>
@@ -554,7 +551,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -630,6 +627,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -731,7 +734,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -747,14 +750,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -767,8 +766,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -818,6 +815,46 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1105,626 +1142,648 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView zoomScale="95" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" customWidth="1"/>
-    <col min="14" max="14" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" hidden="1" customWidth="1"/>
+    <col min="9" max="11" width="8.88671875" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="33" t="s">
+      <c r="E1" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="22">
-        <v>-2</v>
-      </c>
-      <c r="J1" s="22">
-        <v>-1</v>
-      </c>
-      <c r="K1" s="22">
-        <v>0</v>
-      </c>
-      <c r="L1" s="22">
+      <c r="I1" s="63">
+        <v>0</v>
+      </c>
+      <c r="J1" s="63">
+        <v>0.5</v>
+      </c>
+      <c r="K1" s="63">
         <v>1</v>
       </c>
-      <c r="M1" s="22">
-        <v>2</v>
-      </c>
-      <c r="N1" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L1" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="66">
         <v>-1</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="66">
         <v>1</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="17">
+      <c r="F2" s="77">
+        <f>ABS(D2*E2)</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="67">
         <f>IF(E2&lt;0.5, E2, E2*2)</f>
         <v>2</v>
       </c>
-      <c r="H2" s="19">
+      <c r="H2" s="68">
         <f t="shared" ref="H2:H15" si="0">D2*G2</f>
         <v>-2</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="46"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="66">
         <v>1</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="66">
         <v>0.3</v>
       </c>
-      <c r="F3" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="28">
-        <f t="shared" ref="G3:G15" si="1">IF(E3&lt;0.5, E3, E3*2)</f>
+      <c r="F3" s="77">
+        <f t="shared" ref="F3:F7" si="1">ABS(D3*E3)</f>
         <v>0.3</v>
       </c>
-      <c r="H3" s="19">
+      <c r="G3" s="71">
+        <f t="shared" ref="G3:G15" si="2">IF(E3&lt;0.5, E3, E3*2)</f>
+        <v>0.3</v>
+      </c>
+      <c r="H3" s="68">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="46"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I3" s="69"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="66">
         <v>0.39</v>
       </c>
-      <c r="E4" s="28">
-        <v>0</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="28">
+      <c r="E4" s="66">
+        <v>0</v>
+      </c>
+      <c r="F4" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H4" s="19">
+      <c r="G4" s="71">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="46"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I4" s="69"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="66">
         <v>1</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="66">
         <v>1</v>
       </c>
-      <c r="F5" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="17">
+      <c r="F5" s="77">
         <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G5" s="67">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="68">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="46"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="56"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="10">
-        <v>0</v>
-      </c>
-      <c r="E6" s="17">
+      <c r="D6" s="66">
+        <v>0</v>
+      </c>
+      <c r="E6" s="66">
         <v>0.6</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="17">
+      <c r="F6" s="77">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="67">
+        <f t="shared" si="2"/>
         <v>1.2</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="46"/>
-    </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I6" s="69"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="10">
-        <v>0</v>
-      </c>
-      <c r="E7" s="15">
-        <v>0</v>
-      </c>
-      <c r="F7" s="16" t="s">
+      <c r="D7" s="66">
+        <v>0</v>
+      </c>
+      <c r="E7" s="66">
+        <v>0</v>
+      </c>
+      <c r="F7" s="77">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="71">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="68">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="69"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="O7" s="40" t="s">
+      <c r="N7" s="74" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>1</v>
+      </c>
+      <c r="B8" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="76">
+        <v>-1.3959686147186101E-2</v>
+      </c>
+      <c r="E8" s="76">
+        <v>0.43129437229437201</v>
+      </c>
+      <c r="F8" s="77">
+        <f>ABS(D8*E8)</f>
+        <v>6.0207340742770695E-3</v>
+      </c>
+      <c r="G8" s="78">
+        <f t="shared" si="2"/>
+        <v>0.43129437229437201</v>
+      </c>
+      <c r="H8" s="68">
+        <f>D8*G8</f>
+        <v>-6.0207340742770695E-3</v>
+      </c>
+      <c r="I8" s="69"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="79">
+        <v>49.5</v>
+      </c>
+      <c r="M8" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="P7" s="40" t="s">
+      <c r="N8" s="70" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="12">
-        <v>1</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="14">
-        <v>-1.3959686147186101E-2</v>
-      </c>
-      <c r="E8" s="29">
-        <v>0.43129437229437201</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="29">
-        <f t="shared" si="1"/>
-        <v>0.43129437229437201</v>
-      </c>
-      <c r="H8" s="32">
-        <f t="shared" si="0"/>
-        <v>-6.0207340742770695E-3</v>
-      </c>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="43">
-        <v>49.5</v>
-      </c>
-      <c r="O8" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="P8" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="76">
         <v>5.5258047508047498E-2</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="76">
         <v>0.43147743922743897</v>
       </c>
-      <c r="G9" s="11">
-        <f t="shared" si="1"/>
+      <c r="F9" s="77">
+        <f t="shared" ref="F9:F15" si="3">ABS(D9*E9)</f>
+        <v>2.3842600835480499E-2</v>
+      </c>
+      <c r="G9" s="78">
+        <f t="shared" si="2"/>
         <v>0.43147743922743897</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="68">
         <f t="shared" si="0"/>
         <v>2.3842600835480499E-2</v>
       </c>
-      <c r="I9" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="44">
+      <c r="I9" s="69"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="81">
         <v>95</v>
       </c>
-      <c r="O9" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="P9" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M9" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="N9" s="73" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="6">
+      <c r="C10" s="80" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="76">
         <v>0.203059861285667</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="76">
         <v>0.50926139272913395</v>
       </c>
-      <c r="G10" s="17">
-        <f t="shared" si="1"/>
+      <c r="F10" s="77">
+        <f t="shared" si="3"/>
+        <v>0.10341054776572353</v>
+      </c>
+      <c r="G10" s="67">
+        <f t="shared" si="2"/>
         <v>1.0185227854582679</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="68">
         <f t="shared" si="0"/>
         <v>0.20682109553144706</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="45">
+      <c r="I10" s="69"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="79">
         <v>82.5</v>
       </c>
-      <c r="O10" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="P10" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M10" s="70" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="70" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="B11" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="75" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="76">
         <v>8.2133490344480198E-2</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="76">
         <v>0.41494910756655701</v>
       </c>
-      <c r="G11" s="11">
-        <f t="shared" si="1"/>
+      <c r="F11" s="77">
+        <f t="shared" si="3"/>
+        <v>3.4081218519768482E-2</v>
+      </c>
+      <c r="G11" s="78">
+        <f t="shared" si="2"/>
         <v>0.41494910756655701</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="68">
         <f t="shared" si="0"/>
         <v>3.4081218519768482E-2</v>
       </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="44">
+      <c r="I11" s="69"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="81">
         <v>100</v>
       </c>
-      <c r="O11" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="P11" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="25">
+      <c r="M11" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="N11" s="73" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="21">
         <v>5</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="76">
         <v>7.5195158871629406E-2</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="76">
         <v>0.54452720663504905</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="17">
-        <f t="shared" si="1"/>
+      <c r="F12" s="77">
+        <f t="shared" si="3"/>
+        <v>4.0945809812847088E-2</v>
+      </c>
+      <c r="G12" s="67">
+        <f t="shared" si="2"/>
         <v>1.0890544132700981</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="68">
         <f t="shared" si="0"/>
         <v>8.1891619625694176E-2</v>
       </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="45">
+      <c r="I12" s="69"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="79">
         <v>95</v>
       </c>
-      <c r="O12" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="P12" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="41">
+      <c r="M12" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="N12" s="70" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="35">
         <v>6</v>
       </c>
-      <c r="B13" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="6">
+      <c r="B13" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="75" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="76">
         <v>-0.113888888888888</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="76">
         <v>0.65277777777777701</v>
       </c>
-      <c r="G13" s="17">
-        <f t="shared" si="1"/>
+      <c r="F13" s="77">
+        <f t="shared" si="3"/>
+        <v>7.4344135802468472E-2</v>
+      </c>
+      <c r="G13" s="67">
+        <f t="shared" si="2"/>
         <v>1.305555555555554</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="68">
         <f t="shared" si="0"/>
         <v>-0.14868827160493694</v>
       </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="44">
+      <c r="I13" s="69"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="72"/>
+      <c r="L13" s="81">
         <v>100</v>
       </c>
-      <c r="O13" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="P13" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="41">
+      <c r="M13" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="N13" s="73" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="35">
         <v>7</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="82" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="6">
+      <c r="D14" s="76">
         <v>0.14939723320158099</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="76">
         <v>0.37066205533596802</v>
       </c>
-      <c r="G14" s="11">
-        <f t="shared" si="1"/>
+      <c r="F14" s="77">
+        <f t="shared" si="3"/>
+        <v>5.5375885520004935E-2</v>
+      </c>
+      <c r="G14" s="78">
+        <f t="shared" si="2"/>
         <v>0.37066205533596802</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="68">
         <f t="shared" si="0"/>
         <v>5.5375885520004935E-2</v>
       </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="45">
+      <c r="I14" s="69"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="79">
         <v>75</v>
       </c>
-      <c r="O14" s="20" t="s">
+      <c r="M14" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="N14" s="70" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="35">
+        <v>8</v>
+      </c>
+      <c r="B15" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="P14" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="41">
-        <v>8</v>
-      </c>
-      <c r="B15" s="41" t="s">
+      <c r="C15" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="6">
+      <c r="D15" s="76">
         <v>1.4011491728883E-2</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="76">
         <v>0.38156382667252198</v>
       </c>
-      <c r="G15" s="11">
-        <f t="shared" si="1"/>
+      <c r="F15" s="77">
+        <f t="shared" si="3"/>
+        <v>5.3462784014629882E-3</v>
+      </c>
+      <c r="G15" s="78">
+        <f t="shared" si="2"/>
         <v>0.38156382667252198</v>
       </c>
-      <c r="H15" s="19">
+      <c r="H15" s="68">
         <f t="shared" si="0"/>
         <v>5.3462784014629882E-3</v>
       </c>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="44">
+      <c r="I15" s="69"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="72"/>
+      <c r="L15" s="81">
         <v>100</v>
       </c>
-      <c r="O15" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="P15" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M15" s="73" t="s">
+        <v>42</v>
+      </c>
+      <c r="N15" s="73" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C17" s="2"/>
-      <c r="O17" s="31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F18" s="6">
+        <f>SUM(F8:F15)</f>
+        <v>0.34336721073203308</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C19" s="2"/>
-      <c r="I19" s="37">
+      <c r="F19">
+        <f>F18/8</f>
+        <v>4.2920901341504135E-2</v>
+      </c>
+      <c r="I19" s="31">
         <v>-1</v>
       </c>
-      <c r="J19" s="35">
-        <v>0</v>
-      </c>
-      <c r="K19" s="38" t="s">
+      <c r="J19" s="29">
+        <v>0</v>
+      </c>
+      <c r="K19" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="L19" s="36" t="s">
+      <c r="L19" s="30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20" s="2"/>
@@ -1735,9 +1794,8 @@
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20"/>
-      <c r="M20"/>
-    </row>
-    <row r="21" spans="1:15" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:12" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21" s="2"/>
@@ -1745,18 +1803,17 @@
       <c r="G21"/>
       <c r="H21"/>
       <c r="I21"/>
-      <c r="J21" s="37">
-        <v>0</v>
-      </c>
-      <c r="K21" s="38" t="s">
+      <c r="J21" s="31">
+        <v>0</v>
+      </c>
+      <c r="K21" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="L21" s="36" t="s">
+      <c r="L21" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="M21"/>
-    </row>
-    <row r="22" spans="1:15" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:12" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22" s="2"/>
@@ -1767,9 +1824,8 @@
       <c r="J22"/>
       <c r="K22"/>
       <c r="L22"/>
-      <c r="M22"/>
-    </row>
-    <row r="23" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23" s="2"/>
@@ -1777,14 +1833,13 @@
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
-      <c r="J23" s="39" t="s">
+      <c r="J23" s="33" t="s">
         <v>24</v>
       </c>
       <c r="K23"/>
       <c r="L23"/>
-      <c r="M23"/>
-    </row>
-    <row r="24" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24" s="2"/>
@@ -1792,14 +1847,13 @@
       <c r="G24"/>
       <c r="H24"/>
       <c r="I24"/>
-      <c r="J24" s="39" t="s">
+      <c r="J24" s="33" t="s">
         <v>23</v>
       </c>
       <c r="K24"/>
       <c r="L24"/>
-      <c r="M24"/>
-    </row>
-    <row r="25" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25" s="2"/>
@@ -1809,10 +1863,8 @@
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
-      <c r="L25"/>
-      <c r="M25"/>
-    </row>
-    <row r="26" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26" s="2"/>
@@ -1822,10 +1874,8 @@
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
-      <c r="L26"/>
-      <c r="M26"/>
-    </row>
-    <row r="27" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27" s="2"/>
@@ -1835,10 +1885,8 @@
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
-      <c r="L27"/>
-      <c r="M27"/>
-    </row>
-    <row r="28" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28" s="2"/>
@@ -1848,10 +1896,8 @@
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
-      <c r="L28"/>
-      <c r="M28"/>
-    </row>
-    <row r="29" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29" s="2"/>
@@ -1861,10 +1907,8 @@
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
-      <c r="L29"/>
-      <c r="M29"/>
-    </row>
-    <row r="30" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30" s="2"/>
@@ -1874,10 +1918,8 @@
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
-      <c r="L30"/>
-      <c r="M30"/>
-    </row>
-    <row r="31" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31" s="2"/>
@@ -1887,10 +1929,8 @@
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
-      <c r="L31"/>
-      <c r="M31"/>
-    </row>
-    <row r="33" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33" s="2"/>
@@ -1900,10 +1940,8 @@
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
-      <c r="L33"/>
-      <c r="M33"/>
-    </row>
-    <row r="34" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34" s="2"/>
@@ -1913,10 +1951,8 @@
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
-      <c r="L34"/>
-      <c r="M34"/>
-    </row>
-    <row r="35" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35" s="2"/>
@@ -1926,12 +1962,10 @@
       <c r="I35"/>
       <c r="J35"/>
       <c r="K35"/>
-      <c r="L35"/>
-      <c r="M35"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="L1:N1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1"/>
@@ -1987,47 +2021,47 @@
       <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="G1" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="52" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="33" t="s">
+      <c r="H1" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="48" t="s">
-        <v>53</v>
-      </c>
       <c r="I1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J1" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="K1" s="22">
+        <v>56</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="18">
         <v>-2</v>
       </c>
-      <c r="L1" s="22">
+      <c r="L1" s="18">
         <v>-1</v>
       </c>
-      <c r="M1" s="22">
-        <v>0</v>
-      </c>
-      <c r="N1" s="22">
+      <c r="M1" s="18">
+        <v>0</v>
+      </c>
+      <c r="N1" s="18">
         <v>1</v>
       </c>
-      <c r="O1" s="22">
+      <c r="O1" s="18">
         <v>2</v>
       </c>
-      <c r="P1" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
+      <c r="P1" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -2039,34 +2073,34 @@
       <c r="C2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="53">
+      <c r="D2" s="47">
         <v>0.53800000000000003</v>
       </c>
-      <c r="E2" s="53">
+      <c r="E2" s="47">
         <v>0.46200000000000002</v>
       </c>
-      <c r="F2" s="53">
-        <v>0</v>
-      </c>
-      <c r="G2" s="53">
+      <c r="F2" s="47">
+        <v>0</v>
+      </c>
+      <c r="G2" s="47">
         <v>-0.5423</v>
       </c>
-      <c r="H2" s="57" t="s">
-        <v>54</v>
+      <c r="H2" s="51" t="s">
+        <v>52</v>
       </c>
       <c r="I2" s="10">
         <v>-1</v>
       </c>
-      <c r="J2" s="19">
+      <c r="J2" s="15">
         <f t="shared" ref="J2:J15" si="0">F2*I2</f>
         <v>0</v>
       </c>
       <c r="K2" s="7"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="46"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="40"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
@@ -2078,34 +2112,34 @@
       <c r="C3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="53">
-        <v>0</v>
-      </c>
-      <c r="E3" s="53">
+      <c r="D3" s="47">
+        <v>0</v>
+      </c>
+      <c r="E3" s="47">
         <v>0.625</v>
       </c>
-      <c r="F3" s="53">
+      <c r="F3" s="47">
         <v>0.375</v>
       </c>
-      <c r="G3" s="53">
+      <c r="G3" s="47">
         <v>0.63690000000000002</v>
       </c>
-      <c r="H3" s="59" t="s">
-        <v>52</v>
+      <c r="H3" s="53" t="s">
+        <v>50</v>
       </c>
       <c r="I3" s="10">
         <v>1</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="15">
         <f t="shared" si="0"/>
         <v>0.375</v>
       </c>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
       <c r="N3" s="7"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="46"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="40"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
@@ -2117,34 +2151,34 @@
       <c r="C4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="53">
-        <v>0</v>
-      </c>
-      <c r="E4" s="53">
+      <c r="D4" s="47">
+        <v>0</v>
+      </c>
+      <c r="E4" s="47">
         <v>0.68700000000000006</v>
       </c>
-      <c r="F4" s="53">
+      <c r="F4" s="47">
         <v>0.313</v>
       </c>
-      <c r="G4" s="53">
+      <c r="G4" s="47">
         <v>0.49270000000000003</v>
       </c>
-      <c r="H4" s="59" t="s">
-        <v>52</v>
+      <c r="H4" s="53" t="s">
+        <v>50</v>
       </c>
       <c r="I4" s="10">
         <v>0.39</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="15">
         <f t="shared" si="0"/>
         <v>0.12207</v>
       </c>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
       <c r="M4" s="7"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="46"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="40"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
@@ -2156,34 +2190,34 @@
       <c r="C5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="53">
-        <v>0</v>
-      </c>
-      <c r="E5" s="53">
+      <c r="D5" s="47">
+        <v>0</v>
+      </c>
+      <c r="E5" s="47">
         <v>0.51900000000000002</v>
       </c>
-      <c r="F5" s="53">
+      <c r="F5" s="47">
         <v>0.48099999999999998</v>
       </c>
-      <c r="G5" s="53">
+      <c r="G5" s="47">
         <v>0.57189999999999996</v>
       </c>
-      <c r="H5" s="59" t="s">
-        <v>52</v>
+      <c r="H5" s="53" t="s">
+        <v>50</v>
       </c>
       <c r="I5" s="10">
         <v>1</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="15">
         <f t="shared" si="0"/>
         <v>0.48099999999999998</v>
       </c>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
       <c r="O5" s="7"/>
-      <c r="P5" s="46"/>
+      <c r="P5" s="40"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
@@ -2195,34 +2229,34 @@
       <c r="C6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="53">
-        <v>0</v>
-      </c>
-      <c r="E6" s="53">
+      <c r="D6" s="47">
+        <v>0</v>
+      </c>
+      <c r="E6" s="47">
         <v>1</v>
       </c>
-      <c r="F6" s="53">
-        <v>0</v>
-      </c>
-      <c r="G6" s="53">
-        <v>0</v>
-      </c>
-      <c r="H6" s="49" t="s">
-        <v>57</v>
+      <c r="F6" s="47">
+        <v>0</v>
+      </c>
+      <c r="G6" s="47">
+        <v>0</v>
+      </c>
+      <c r="H6" s="43" t="s">
+        <v>54</v>
       </c>
       <c r="I6" s="10">
         <v>0</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
       <c r="M6" s="7"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="46"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="40"/>
     </row>
     <row r="7" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
@@ -2234,88 +2268,88 @@
       <c r="C7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="53">
-        <v>0</v>
-      </c>
-      <c r="E7" s="53">
+      <c r="D7" s="47">
+        <v>0</v>
+      </c>
+      <c r="E7" s="47">
         <v>0.84</v>
       </c>
-      <c r="F7" s="53">
+      <c r="F7" s="47">
         <v>0.16</v>
       </c>
-      <c r="G7" s="53">
+      <c r="G7" s="47">
         <v>0.2263</v>
       </c>
-      <c r="H7" s="59" t="s">
-        <v>52</v>
+      <c r="H7" s="53" t="s">
+        <v>50</v>
       </c>
       <c r="I7" s="10">
         <v>0</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
       <c r="M7" s="7"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q7" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="R7" s="40" t="s">
-        <v>30</v>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q7" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="R7" s="34" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="54">
+      <c r="A8" s="48">
         <v>1</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="56">
+      <c r="D8" s="50">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="E8" s="56">
+      <c r="E8" s="50">
         <v>0.82</v>
       </c>
-      <c r="F8" s="56">
+      <c r="F8" s="50">
         <v>0.122</v>
       </c>
-      <c r="G8" s="56">
+      <c r="G8" s="50">
         <v>0.98270000000000002</v>
       </c>
-      <c r="H8" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="I8" s="14">
+      <c r="H8" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="12">
         <v>-1.3959686147186101E-2</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="26">
         <f t="shared" si="0"/>
         <v>-1.7030817099567043E-3</v>
       </c>
-      <c r="K8" s="23"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="43">
+      <c r="K8" s="19"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="37">
         <v>49.5</v>
       </c>
-      <c r="Q8" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="R8" s="23" t="s">
-        <v>32</v>
+      <c r="Q8" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8" s="19" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -2326,43 +2360,43 @@
         <v>3</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="53">
+        <v>55</v>
+      </c>
+      <c r="D9" s="47">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="E9" s="53">
+      <c r="E9" s="47">
         <v>0.86199999999999999</v>
       </c>
-      <c r="F9" s="53">
+      <c r="F9" s="47">
         <v>6.2E-2</v>
       </c>
-      <c r="G9" s="53">
+      <c r="G9" s="47">
         <v>-0.9819</v>
       </c>
-      <c r="H9" s="57" t="s">
-        <v>54</v>
+      <c r="H9" s="51" t="s">
+        <v>52</v>
       </c>
       <c r="I9" s="6">
         <v>5.5258047508047498E-2</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="15">
         <f t="shared" si="0"/>
         <v>3.4259989454989447E-3</v>
       </c>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
       <c r="N9" s="7"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="44">
+      <c r="O9" s="17"/>
+      <c r="P9" s="38">
         <v>95</v>
       </c>
-      <c r="Q9" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="R9" s="31" t="s">
-        <v>32</v>
+      <c r="Q9" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="R9" s="25" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -2373,43 +2407,43 @@
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="53">
+        <v>53</v>
+      </c>
+      <c r="D10" s="47">
         <v>2.7E-2</v>
       </c>
-      <c r="E10" s="53">
+      <c r="E10" s="47">
         <v>0.92300000000000004</v>
       </c>
-      <c r="F10" s="53">
+      <c r="F10" s="47">
         <v>0.05</v>
       </c>
-      <c r="G10" s="53">
+      <c r="G10" s="47">
         <v>0.89629999999999999</v>
       </c>
-      <c r="H10" s="59" t="s">
-        <v>52</v>
+      <c r="H10" s="53" t="s">
+        <v>50</v>
       </c>
       <c r="I10" s="6">
         <v>0.203059861285667</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="15">
         <f t="shared" si="0"/>
         <v>1.015299306428335E-2</v>
       </c>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
       <c r="N10" s="7"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="45">
+      <c r="O10" s="16"/>
+      <c r="P10" s="39">
         <v>82.5</v>
       </c>
-      <c r="Q10" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="R10" s="20" t="s">
-        <v>32</v>
+      <c r="Q10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="R10" s="16" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -2417,268 +2451,268 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="53">
+        <v>32</v>
+      </c>
+      <c r="D11" s="47">
         <v>0.112</v>
       </c>
-      <c r="E11" s="53">
+      <c r="E11" s="47">
         <v>0.81200000000000006</v>
       </c>
-      <c r="F11" s="53">
+      <c r="F11" s="47">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="G11" s="53">
+      <c r="G11" s="47">
         <v>-0.99660000000000004</v>
       </c>
-      <c r="H11" s="57" t="s">
-        <v>54</v>
+      <c r="H11" s="51" t="s">
+        <v>52</v>
       </c>
       <c r="I11" s="6">
         <v>8.2133490344480198E-2</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="15">
         <f t="shared" si="0"/>
         <v>6.3242787565249755E-3</v>
       </c>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
       <c r="N11" s="7"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="44">
+      <c r="O11" s="17"/>
+      <c r="P11" s="38">
         <v>100</v>
       </c>
-      <c r="Q11" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="R11" s="31" t="s">
-        <v>32</v>
+      <c r="Q11" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="R11" s="25" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="25">
+      <c r="A12" s="21">
         <v>5</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="53">
+      <c r="D12" s="47">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="E12" s="53">
+      <c r="E12" s="47">
         <v>0.77900000000000003</v>
       </c>
-      <c r="F12" s="53">
+      <c r="F12" s="47">
         <v>0.128</v>
       </c>
-      <c r="G12" s="53">
+      <c r="G12" s="47">
         <v>0.99790000000000001</v>
       </c>
-      <c r="H12" s="59" t="s">
-        <v>52</v>
+      <c r="H12" s="53" t="s">
+        <v>50</v>
       </c>
       <c r="I12" s="6">
         <v>7.5195158871629406E-2</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="15">
         <f t="shared" si="0"/>
         <v>9.6249803355685642E-3</v>
       </c>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="45">
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="39">
         <v>95</v>
       </c>
-      <c r="Q12" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="R12" s="20" t="s">
-        <v>32</v>
+      <c r="Q12" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="R12" s="16" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="41">
+      <c r="A13" s="35">
         <v>6</v>
       </c>
-      <c r="B13" s="41" t="s">
-        <v>37</v>
+      <c r="B13" s="35" t="s">
+        <v>35</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="53">
+        <v>36</v>
+      </c>
+      <c r="D13" s="47">
         <v>0.09</v>
       </c>
-      <c r="E13" s="53">
+      <c r="E13" s="47">
         <v>0.76</v>
       </c>
-      <c r="F13" s="53">
+      <c r="F13" s="47">
         <v>0.14899999999999999</v>
       </c>
-      <c r="G13" s="53">
+      <c r="G13" s="47">
         <v>0.93859999999999999</v>
       </c>
-      <c r="H13" s="59" t="s">
-        <v>52</v>
+      <c r="H13" s="53" t="s">
+        <v>50</v>
       </c>
       <c r="I13" s="6">
         <v>-0.113888888888888</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J13" s="15">
         <f t="shared" si="0"/>
         <v>-1.6969444444444311E-2</v>
       </c>
-      <c r="K13" s="21"/>
+      <c r="K13" s="17"/>
       <c r="L13" s="7"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="44">
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="38">
         <v>100</v>
       </c>
-      <c r="Q13" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="R13" s="31" t="s">
-        <v>32</v>
+      <c r="Q13" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="R13" s="25" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="41">
+      <c r="A14" s="35">
         <v>7</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="53">
+      <c r="D14" s="47">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="E14" s="53">
+      <c r="E14" s="47">
         <v>0.85599999999999998</v>
       </c>
-      <c r="F14" s="53">
+      <c r="F14" s="47">
         <v>0.109</v>
       </c>
-      <c r="G14" s="53">
+      <c r="G14" s="47">
         <v>0.995</v>
       </c>
-      <c r="H14" s="59" t="s">
-        <v>52</v>
+      <c r="H14" s="53" t="s">
+        <v>50</v>
       </c>
       <c r="I14" s="6">
         <v>0.14939723320158099</v>
       </c>
-      <c r="J14" s="19">
+      <c r="J14" s="15">
         <f t="shared" si="0"/>
         <v>1.6284298418972328E-2</v>
       </c>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
       <c r="N14" s="7"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="45">
+      <c r="O14" s="16"/>
+      <c r="P14" s="39">
         <v>75</v>
       </c>
-      <c r="Q14" s="20" t="s">
+      <c r="Q14" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="R14" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="35">
+        <v>8</v>
+      </c>
+      <c r="B15" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="R14" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="41">
-        <v>8</v>
-      </c>
-      <c r="B15" s="41" t="s">
+      <c r="C15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="53">
+      <c r="D15" s="47">
         <v>0.123</v>
       </c>
-      <c r="E15" s="53">
+      <c r="E15" s="47">
         <v>0.754</v>
       </c>
-      <c r="F15" s="53">
+      <c r="F15" s="47">
         <v>0.122</v>
       </c>
-      <c r="G15" s="53">
+      <c r="G15" s="47">
         <v>-0.6915</v>
       </c>
-      <c r="H15" s="57" t="s">
-        <v>54</v>
+      <c r="H15" s="51" t="s">
+        <v>52</v>
       </c>
       <c r="I15" s="6">
         <v>1.4011491728883E-2</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J15" s="15">
         <f t="shared" si="0"/>
         <v>1.709401990923726E-3</v>
       </c>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
       <c r="N15" s="7"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="44">
+      <c r="O15" s="17"/>
+      <c r="P15" s="38">
         <v>100</v>
       </c>
-      <c r="Q15" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="R15" s="31" t="s">
-        <v>32</v>
+      <c r="Q15" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="R15" s="25" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C16" s="2"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C17" s="2"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="Q17" s="31" t="s">
-        <v>47</v>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="Q17" s="25" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C18" s="2"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C19" s="2"/>
@@ -2941,7 +2975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
@@ -2966,31 +3000,31 @@
         <v>19</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="46" t="s">
         <v>48</v>
-      </c>
-      <c r="K1" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" s="52" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -2998,28 +3032,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="10">
         <v>1</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="14">
         <v>1</v>
       </c>
-      <c r="G2" s="60">
+      <c r="G2" s="54">
         <v>0.57189999999999996</v>
       </c>
-      <c r="H2" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="53">
-        <v>0</v>
-      </c>
-      <c r="K2" s="53">
+      <c r="H2" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="47">
+        <v>0</v>
+      </c>
+      <c r="K2" s="47">
         <v>0.51900000000000002</v>
       </c>
-      <c r="L2" s="53">
+      <c r="L2" s="47">
         <v>0.48099999999999998</v>
       </c>
     </row>
@@ -3028,31 +3062,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="10">
         <v>-1</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="14">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="60">
+        <v>59</v>
+      </c>
+      <c r="G3" s="54">
         <v>-0.5423</v>
       </c>
-      <c r="H3" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="J3" s="53">
+      <c r="H3" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="47">
         <v>0.53800000000000003</v>
       </c>
-      <c r="K3" s="53">
+      <c r="K3" s="47">
         <v>0.46200000000000002</v>
       </c>
-      <c r="L3" s="53">
+      <c r="L3" s="47">
         <v>0</v>
       </c>
     </row>
@@ -3061,31 +3095,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="10">
         <v>0.39</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="24">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" s="60">
+        <v>60</v>
+      </c>
+      <c r="G4" s="54">
         <v>0.49270000000000003</v>
       </c>
-      <c r="H4" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="J4" s="53">
-        <v>0</v>
-      </c>
-      <c r="K4" s="53">
+      <c r="H4" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="47">
+        <v>0</v>
+      </c>
+      <c r="K4" s="47">
         <v>0.68700000000000006</v>
       </c>
-      <c r="L4" s="53">
+      <c r="L4" s="47">
         <v>0.313</v>
       </c>
     </row>
@@ -3094,28 +3128,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="10">
         <v>0</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="14">
         <v>0.6</v>
       </c>
-      <c r="G5" s="60">
-        <v>0</v>
-      </c>
-      <c r="H5" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="J5" s="53">
-        <v>0</v>
-      </c>
-      <c r="K5" s="53">
+      <c r="G5" s="54">
+        <v>0</v>
+      </c>
+      <c r="H5" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="47">
+        <v>0</v>
+      </c>
+      <c r="K5" s="47">
         <v>1</v>
       </c>
-      <c r="L5" s="53">
+      <c r="L5" s="47">
         <v>0</v>
       </c>
     </row>
@@ -3124,70 +3158,70 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="10">
         <v>0</v>
       </c>
-      <c r="E6" s="15">
-        <v>0</v>
-      </c>
-      <c r="G6" s="60">
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="G6" s="54">
         <v>0.2263</v>
       </c>
-      <c r="H6" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" s="53">
-        <v>0</v>
-      </c>
-      <c r="K6" s="53">
+      <c r="H6" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="47">
+        <v>0</v>
+      </c>
+      <c r="K6" s="47">
         <v>0.84</v>
       </c>
-      <c r="L6" s="53">
+      <c r="L6" s="47">
         <v>0.16</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="63" t="s">
-        <v>111</v>
-      </c>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
+      <c r="B21" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="63" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
+      <c r="B22" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="63" t="s">
-        <v>113</v>
-      </c>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
+      <c r="B23" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3211,155 +3245,155 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="61" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="56" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="62" t="s">
+      <c r="B3" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="62" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="56" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="62" t="s">
+      <c r="B4" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="62" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="56" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="62" t="s">
+      <c r="B5" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="62" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="56" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="62" t="s">
+      <c r="B6" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="62" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="56" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="62" t="s">
+      <c r="B7" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="62" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="56" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="62" t="s">
+      <c r="B8" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="62" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="56" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="62" t="s">
+      <c r="B9" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="62" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="56" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="62" t="s">
+      <c r="B10" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="62" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="56" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="62" t="s">
+      <c r="B11" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="62" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="56" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="62" t="s">
+      <c r="B12" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="62" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="56" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="62" t="s">
+      <c r="B13" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="62" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="56" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="62" t="s">
+      <c r="B14" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="62" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="56" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="62" t="s">
+      <c r="B15" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="62" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="56" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="62" t="s">
+      <c r="B16" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="62" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="56" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="62" t="s">
+      <c r="B17" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="62" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="56" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="62" t="s">
+      <c r="B18" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="62" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="56" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="62" t="s">
+      <c r="B19" s="56" t="s">
         <v>107</v>
-      </c>
-      <c r="B18" s="62" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="62" t="s">
-        <v>109</v>
-      </c>
-      <c r="B19" s="62" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HTTPS added to URL and changed test_lambda_handler
</commit_message>
<xml_diff>
--- a/Docs/Bias_Score_Analysis/Bias Score.xlsx
+++ b/Docs/Bias_Score_Analysis/Bias Score.xlsx
@@ -13,9 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="TEXTBLOB" sheetId="3" r:id="rId1"/>
-    <sheet name="VADER" sheetId="4" r:id="rId2"/>
-    <sheet name="COMPARING" sheetId="5" r:id="rId3"/>
-    <sheet name="SPACY Names Entity Recognition" sheetId="6" r:id="rId4"/>
+    <sheet name="BIAS numbers" sheetId="7" r:id="rId2"/>
+    <sheet name="VADER" sheetId="4" r:id="rId3"/>
+    <sheet name="COMPARING" sheetId="5" r:id="rId4"/>
+    <sheet name="SPACY Names Entity Recognition" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +33,7 @@
     <author>Ana Potje</author>
   </authors>
   <commentList>
-    <comment ref="C17" authorId="0" shapeId="0">
+    <comment ref="C18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="127">
   <si>
     <t>Website</t>
   </si>
@@ -454,6 +455,48 @@
   </si>
   <si>
     <t>Subjectiv</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Neutral(UNS)</t>
+  </si>
+  <si>
+    <t>BiasIndicator</t>
+  </si>
+  <si>
+    <t>Incredibility%</t>
+  </si>
+  <si>
+    <t>Polarity%</t>
+  </si>
+  <si>
+    <t>Subjectivity%</t>
+  </si>
+  <si>
+    <t>https://www.nbcnews.com/news/us-news/canadian-woman-charged-sending-ricin-laced-letter-white-house-n1240760</t>
+  </si>
+  <si>
+    <t>NBC News</t>
+  </si>
+  <si>
+    <t>Wall St Journal</t>
+  </si>
+  <si>
+    <t>BIAS IND</t>
+  </si>
+  <si>
+    <t>POL</t>
+  </si>
+  <si>
+    <t>SUBJ</t>
   </si>
 </sst>
 </file>
@@ -464,7 +507,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -550,8 +593,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -633,6 +699,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,7 +812,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -855,12 +933,32 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1142,10 +1240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1164,7 +1262,7 @@
     <col min="14" max="14" width="20.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -1198,13 +1296,13 @@
       <c r="K1" s="63">
         <v>1</v>
       </c>
-      <c r="L1" s="83" t="s">
+      <c r="L1" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1229,7 +1327,7 @@
         <v>2</v>
       </c>
       <c r="H2" s="68">
-        <f t="shared" ref="H2:H15" si="0">D2*G2</f>
+        <f t="shared" ref="H2:H17" si="0">D2*G2</f>
         <v>-2</v>
       </c>
       <c r="I2" s="70"/>
@@ -1239,7 +1337,7 @@
       <c r="M2" s="56"/>
       <c r="N2" s="56"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1260,7 +1358,7 @@
         <v>0.3</v>
       </c>
       <c r="G3" s="71">
-        <f t="shared" ref="G3:G15" si="2">IF(E3&lt;0.5, E3, E3*2)</f>
+        <f t="shared" ref="G3:G17" si="2">IF(E3&lt;0.5, E3, E3*2)</f>
         <v>0.3</v>
       </c>
       <c r="H3" s="68">
@@ -1274,7 +1372,7 @@
       <c r="M3" s="56"/>
       <c r="N3" s="56"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1309,7 +1407,7 @@
       <c r="M4" s="56"/>
       <c r="N4" s="56"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1344,7 +1442,7 @@
       <c r="M5" s="56"/>
       <c r="N5" s="56"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1379,7 +1477,7 @@
       <c r="M6" s="56"/>
       <c r="N6" s="56"/>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1420,7 +1518,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>1</v>
       </c>
@@ -1461,7 +1559,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1472,22 +1570,22 @@
         <v>12</v>
       </c>
       <c r="D9" s="76">
-        <v>5.5258047508047498E-2</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E9" s="76">
-        <v>0.43147743922743897</v>
+        <v>0.75</v>
       </c>
       <c r="F9" s="77">
-        <f t="shared" ref="F9:F15" si="3">ABS(D9*E9)</f>
-        <v>2.3842600835480499E-2</v>
+        <f t="shared" ref="F9:F17" si="3">ABS(D9*E9)</f>
+        <v>0.41250000000000003</v>
       </c>
       <c r="G9" s="78">
         <f t="shared" si="2"/>
-        <v>0.43147743922743897</v>
+        <v>1.5</v>
       </c>
       <c r="H9" s="68">
         <f t="shared" si="0"/>
-        <v>2.3842600835480499E-2</v>
+        <v>0.82500000000000007</v>
       </c>
       <c r="I9" s="69"/>
       <c r="J9" s="72"/>
@@ -1501,8 +1599,14 @@
       <c r="N9" s="73" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O9" s="76">
+        <v>5.5258047508047498E-2</v>
+      </c>
+      <c r="P9" s="76">
+        <v>0.43147743922743897</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1543,7 +1647,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1584,7 +1688,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="21">
         <v>5</v>
       </c>
@@ -1625,7 +1729,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="35">
         <v>6</v>
       </c>
@@ -1666,7 +1770,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="35">
         <v>7</v>
       </c>
@@ -1707,7 +1811,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="35">
         <v>8</v>
       </c>
@@ -1748,46 +1852,105 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C16" s="2"/>
-      <c r="M16" t="s">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="35">
+        <v>9</v>
+      </c>
+      <c r="B16" s="82" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="75" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="76">
+        <v>-0.113888888888888</v>
+      </c>
+      <c r="E16" s="76">
+        <v>0.65277777777777701</v>
+      </c>
+      <c r="F16" s="77">
+        <f t="shared" si="3"/>
+        <v>7.4344135802468472E-2</v>
+      </c>
+      <c r="G16" s="78">
+        <f t="shared" si="2"/>
+        <v>1.305555555555554</v>
+      </c>
+      <c r="H16" s="68">
+        <f t="shared" si="0"/>
+        <v>-0.14868827160493694</v>
+      </c>
+      <c r="I16" s="69"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="79">
+        <v>100</v>
+      </c>
+      <c r="M16" s="70" t="s">
+        <v>37</v>
+      </c>
+      <c r="N16" s="70" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="35">
+        <v>10</v>
+      </c>
+      <c r="B17" s="82" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="75" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="76">
+        <v>-4.6196660482374703E-2</v>
+      </c>
+      <c r="E17" s="76">
+        <v>0.34431045145330802</v>
+      </c>
+      <c r="F17" s="77">
+        <f t="shared" si="3"/>
+        <v>1.5905993026321629E-2</v>
+      </c>
+      <c r="G17" s="78">
+        <f t="shared" si="2"/>
+        <v>0.34431045145330802</v>
+      </c>
+      <c r="H17" s="68">
+        <f t="shared" si="0"/>
+        <v>-1.5905993026321629E-2</v>
+      </c>
+      <c r="I17" s="69"/>
+      <c r="J17" s="72"/>
+      <c r="K17" s="72"/>
+      <c r="L17" s="81">
+        <v>100</v>
+      </c>
+      <c r="M17" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="N17" s="73" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C18" s="2"/>
+      <c r="M18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C18" s="2"/>
-      <c r="F18" s="6">
-        <f>SUM(F8:F15)</f>
-        <v>0.34336721073203308</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C19" s="2"/>
-      <c r="F19">
-        <f>F18/8</f>
-        <v>4.2920901341504135E-2</v>
-      </c>
-      <c r="I19" s="31">
-        <v>-1</v>
-      </c>
-      <c r="J19" s="29">
-        <v>0</v>
-      </c>
-      <c r="K19" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20" s="2"/>
-      <c r="F20"/>
+      <c r="F20" s="6">
+        <f>SUM(F8:F15)</f>
+        <v>0.7320246098965526</v>
+      </c>
       <c r="G20"/>
       <c r="H20"/>
       <c r="I20"/>
@@ -1795,25 +1958,30 @@
       <c r="K20"/>
       <c r="L20"/>
     </row>
-    <row r="21" spans="1:12" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21" s="2"/>
-      <c r="F21"/>
+      <c r="F21">
+        <f>F20/8</f>
+        <v>9.1503076237069075E-2</v>
+      </c>
       <c r="G21"/>
       <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21" s="31">
+      <c r="I21" s="31">
+        <v>-1</v>
+      </c>
+      <c r="J21" s="29">
         <v>0</v>
       </c>
       <c r="K21" s="32" t="s">
         <v>21</v>
       </c>
       <c r="L21" s="30" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22" s="2"/>
@@ -1825,7 +1993,7 @@
       <c r="K22"/>
       <c r="L22"/>
     </row>
-    <row r="23" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23" s="2"/>
@@ -1833,13 +2001,17 @@
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
-      <c r="J23" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="K23"/>
-      <c r="L23"/>
-    </row>
-    <row r="24" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J23" s="31">
+        <v>0</v>
+      </c>
+      <c r="K23" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24" s="2"/>
@@ -1847,13 +2019,11 @@
       <c r="G24"/>
       <c r="H24"/>
       <c r="I24"/>
-      <c r="J24" s="33" t="s">
-        <v>23</v>
-      </c>
+      <c r="J24"/>
       <c r="K24"/>
       <c r="L24"/>
     </row>
-    <row r="25" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25" s="2"/>
@@ -1861,10 +2031,13 @@
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25"/>
-      <c r="J25"/>
+      <c r="J25" s="33" t="s">
+        <v>24</v>
+      </c>
       <c r="K25"/>
-    </row>
-    <row r="26" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L25"/>
+    </row>
+    <row r="26" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26" s="2"/>
@@ -1872,10 +2045,13 @@
       <c r="G26"/>
       <c r="H26"/>
       <c r="I26"/>
-      <c r="J26"/>
+      <c r="J26" s="33" t="s">
+        <v>23</v>
+      </c>
       <c r="K26"/>
-    </row>
-    <row r="27" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L26"/>
+    </row>
+    <row r="27" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27" s="2"/>
@@ -1886,7 +2062,7 @@
       <c r="J27"/>
       <c r="K27"/>
     </row>
-    <row r="28" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28" s="2"/>
@@ -1897,7 +2073,7 @@
       <c r="J28"/>
       <c r="K28"/>
     </row>
-    <row r="29" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29" s="2"/>
@@ -1908,7 +2084,7 @@
       <c r="J29"/>
       <c r="K29"/>
     </row>
-    <row r="30" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30" s="2"/>
@@ -1919,7 +2095,7 @@
       <c r="J30"/>
       <c r="K30"/>
     </row>
-    <row r="31" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31" s="2"/>
@@ -1976,14 +2152,446 @@
     <hyperlink ref="C13" r:id="rId6"/>
     <hyperlink ref="C14" r:id="rId7"/>
     <hyperlink ref="C15" r:id="rId8"/>
+    <hyperlink ref="C17" r:id="rId9"/>
+    <hyperlink ref="C16" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
-  <legacyDrawing r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" customWidth="1"/>
+    <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5546875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="91"/>
+    <col min="19" max="19" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="61" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="58" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="83" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="88" t="s">
+        <v>117</v>
+      </c>
+      <c r="L1" s="88" t="s">
+        <v>118</v>
+      </c>
+      <c r="M1" s="88" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q1" s="84" t="s">
+        <v>125</v>
+      </c>
+      <c r="R1" s="84" t="s">
+        <v>126</v>
+      </c>
+      <c r="S1" s="84" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="76">
+        <v>-1.3959686147186101E-2</v>
+      </c>
+      <c r="D2" s="76">
+        <v>0.43129437229437201</v>
+      </c>
+      <c r="E2" s="95">
+        <f>ABS(C2*D2)</f>
+        <v>6.0207340742770695E-3</v>
+      </c>
+      <c r="F2" s="93">
+        <f t="shared" ref="F2:F5" si="0">IF(D2&lt;0.5, D2, D2*2)</f>
+        <v>0.43129437229437201</v>
+      </c>
+      <c r="G2" s="94">
+        <f>C2*F2</f>
+        <v>-6.0207340742770695E-3</v>
+      </c>
+      <c r="H2" s="79">
+        <v>49.5</v>
+      </c>
+      <c r="I2" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="97">
+        <v>31.6751</v>
+      </c>
+      <c r="L2" s="96">
+        <v>54.752400000000002</v>
+      </c>
+      <c r="M2" s="96">
+        <v>-1.51352</v>
+      </c>
+      <c r="N2" s="96">
+        <v>46.761200000000002</v>
+      </c>
+      <c r="O2" s="92">
+        <f>SUM(L2:N2)</f>
+        <v>100.00008</v>
+      </c>
+      <c r="P2" s="89"/>
+      <c r="Q2" s="76">
+        <v>-1.3959686147186101E-2</v>
+      </c>
+      <c r="R2" s="76">
+        <v>0.43129437229437201</v>
+      </c>
+      <c r="S2" s="99">
+        <f t="shared" ref="S2:S5" si="1">(ABS(Q2*100) + (R2*100)+(100-H2))/3</f>
+        <v>31.67513528138527</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="80" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="76">
+        <v>5.5258047508047498E-2</v>
+      </c>
+      <c r="D3" s="76">
+        <v>0.43147743922743897</v>
+      </c>
+      <c r="E3" s="95">
+        <f t="shared" ref="E3:E5" si="2">ABS(C3*D3)</f>
+        <v>2.3842600835480499E-2</v>
+      </c>
+      <c r="F3" s="93">
+        <f t="shared" si="0"/>
+        <v>0.43147743922743897</v>
+      </c>
+      <c r="G3" s="94">
+        <f t="shared" ref="G3:G5" si="3">C3*F3</f>
+        <v>2.3842600835480499E-2</v>
+      </c>
+      <c r="H3" s="79">
+        <v>95</v>
+      </c>
+      <c r="I3" s="70" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" s="73" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="98">
+        <v>45</v>
+      </c>
+      <c r="L3" s="96">
+        <v>3.7037</v>
+      </c>
+      <c r="M3" s="96">
+        <v>40.740699999999997</v>
+      </c>
+      <c r="N3" s="96">
+        <v>55.555599999999998</v>
+      </c>
+      <c r="O3" s="92">
+        <f>SUM(L3:N3)</f>
+        <v>100</v>
+      </c>
+      <c r="Q3" s="76">
+        <v>5.5258047508047498E-2</v>
+      </c>
+      <c r="R3" s="76">
+        <v>0.43147743922743897</v>
+      </c>
+      <c r="S3" s="99">
+        <f>(ABS(Q3*100) + (R3*100)+(100-H3))/3</f>
+        <v>17.891182891182883</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="80" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="76">
+        <v>0.203059861285667</v>
+      </c>
+      <c r="D4" s="76">
+        <v>0.50926139272913395</v>
+      </c>
+      <c r="E4" s="95">
+        <f t="shared" si="2"/>
+        <v>0.10341054776572353</v>
+      </c>
+      <c r="F4" s="93">
+        <f t="shared" si="0"/>
+        <v>1.0185227854582679</v>
+      </c>
+      <c r="G4" s="94">
+        <f t="shared" si="3"/>
+        <v>0.20682109553144706</v>
+      </c>
+      <c r="H4" s="79">
+        <v>82.5</v>
+      </c>
+      <c r="I4" s="70" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="90">
+        <v>29.461400000000001</v>
+      </c>
+      <c r="L4" s="96">
+        <v>19.799900000000001</v>
+      </c>
+      <c r="M4" s="96">
+        <v>21.4695</v>
+      </c>
+      <c r="N4" s="96">
+        <v>58.730600000000003</v>
+      </c>
+      <c r="O4" s="92">
+        <f>SUM(L4:N4)</f>
+        <v>100</v>
+      </c>
+      <c r="Q4" s="76">
+        <v>0.203059861285667</v>
+      </c>
+      <c r="R4" s="76">
+        <v>0.50926139272913395</v>
+      </c>
+      <c r="S4" s="99">
+        <f t="shared" si="1"/>
+        <v>29.577375133826695</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="82" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="75" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="76">
+        <v>0.14939723320158099</v>
+      </c>
+      <c r="D5" s="76">
+        <v>0.37066205533596802</v>
+      </c>
+      <c r="E5" s="95">
+        <f t="shared" si="2"/>
+        <v>5.5375885520004935E-2</v>
+      </c>
+      <c r="F5" s="93">
+        <f t="shared" si="0"/>
+        <v>0.37066205533596802</v>
+      </c>
+      <c r="G5" s="94">
+        <f t="shared" si="3"/>
+        <v>5.5375885520004935E-2</v>
+      </c>
+      <c r="H5" s="79">
+        <v>75</v>
+      </c>
+      <c r="I5" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="90">
+        <v>25.668600000000001</v>
+      </c>
+      <c r="L5" s="96">
+        <v>32.465000000000003</v>
+      </c>
+      <c r="M5" s="96">
+        <v>19.400700000000001</v>
+      </c>
+      <c r="N5" s="96">
+        <v>48.1342</v>
+      </c>
+      <c r="O5" s="92">
+        <f>SUM(L5:N5)</f>
+        <v>99.999899999999997</v>
+      </c>
+      <c r="Q5" s="76">
+        <v>0.14939723320158099</v>
+      </c>
+      <c r="R5" s="76">
+        <v>0.37066205533596802</v>
+      </c>
+      <c r="S5" s="99">
+        <f t="shared" si="1"/>
+        <v>25.668642951251638</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="82" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="75" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="95">
+        <v>7.4344135802468472E-2</v>
+      </c>
+      <c r="H6" s="79">
+        <v>100</v>
+      </c>
+      <c r="I6" s="70" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="90">
+        <v>25.555599999999998</v>
+      </c>
+      <c r="L6" s="96">
+        <v>0</v>
+      </c>
+      <c r="M6" s="96">
+        <v>-21.134</v>
+      </c>
+      <c r="N6" s="96">
+        <v>121.134</v>
+      </c>
+      <c r="O6" s="92">
+        <f>SUM(L6:N6)</f>
+        <v>100</v>
+      </c>
+      <c r="Q6" s="76">
+        <v>-0.113888888888888</v>
+      </c>
+      <c r="R6" s="76">
+        <v>0.65277777777777701</v>
+      </c>
+      <c r="S6" s="99">
+        <f>(ABS(Q6*100) + (R6*100)+(100-H6))/3</f>
+        <v>25.5555555555555</v>
+      </c>
+      <c r="T6" s="6"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="82" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="75" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="95">
+        <v>1.5905993026321629E-2</v>
+      </c>
+      <c r="H7" s="79">
+        <v>100</v>
+      </c>
+      <c r="I7" s="70" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="90">
+        <v>13.0169</v>
+      </c>
+      <c r="L7" s="96">
+        <v>0</v>
+      </c>
+      <c r="M7" s="96">
+        <v>-15.4963</v>
+      </c>
+      <c r="N7" s="96">
+        <v>115.496</v>
+      </c>
+      <c r="O7" s="92">
+        <f>SUM(L7:N7)</f>
+        <v>99.99969999999999</v>
+      </c>
+      <c r="Q7" s="76">
+        <v>-4.6196660482374703E-2</v>
+      </c>
+      <c r="R7" s="76">
+        <v>0.34431045145330802</v>
+      </c>
+      <c r="S7" s="99">
+        <f>(ABS(Q7*100) + (R7*100)+(100-H7))/3</f>
+        <v>13.016903731189423</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B6" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R35"/>
   <sheetViews>
@@ -2057,11 +2665,11 @@
       <c r="O1" s="18">
         <v>2</v>
       </c>
-      <c r="P1" s="84" t="s">
+      <c r="P1" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="85"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -2971,7 +3579,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
@@ -3230,7 +3838,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>

</xml_diff>